<commit_message>
Nieuwe factuur en software update
</commit_message>
<xml_diff>
--- a/Onderdelen en kosten.xlsx
+++ b/Onderdelen en kosten.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
   <si>
     <t>Aantal</t>
   </si>
@@ -266,6 +266,15 @@
   </si>
   <si>
     <t>Prijs inclusief wisselkosten</t>
+  </si>
+  <si>
+    <t>allekabels.nl</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Plastic-spray</t>
   </si>
 </sst>
 </file>
@@ -665,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -731,7 +740,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="3">
-        <f t="shared" ref="E2:E28" si="0">A2*D2</f>
+        <f t="shared" ref="E2:E29" si="0">A2*D2</f>
         <v>100</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1168,491 +1177,511 @@
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19">
-        <v>1</v>
-      </c>
       <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="17">
+        <v>2</v>
+      </c>
+      <c r="H19" s="22">
+        <v>22.93</v>
+      </c>
+      <c r="J19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3">
         <v>15</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E20" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G19" s="17">
-        <v>1</v>
-      </c>
-      <c r="H19" s="3">
+      <c r="G20" s="17">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
         <v>13.16</v>
       </c>
-      <c r="I19" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="B20" t="s">
+      <c r="I20" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="B21" t="s">
         <v>34</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="17">
-        <v>1</v>
-      </c>
-      <c r="H20" s="22">
+      <c r="G21" s="17">
+        <v>1</v>
+      </c>
+      <c r="H21" s="22">
         <f>(7.44+7.4/2)*1.21</f>
         <v>13.4794</v>
       </c>
-      <c r="I20" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="I21" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
         <v>35</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="3">
-        <v>9</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="D22" s="3">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G22" s="17">
         <v>2</v>
       </c>
-      <c r="H21" s="23">
+      <c r="H22" s="23">
         <f>18+8.95/2</f>
         <v>22.475000000000001</v>
       </c>
-      <c r="I21" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22">
+      <c r="I22" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>4</v>
       </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="3">
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3">
         <f>2.5/10/25*30</f>
         <v>0.3</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E23" s="3">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G23" s="17">
         <v>50</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H23" s="3">
         <v>4.92</v>
       </c>
-      <c r="I22" s="17">
+      <c r="I23" s="17">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23">
+    <row r="24" spans="1:10">
+      <c r="A24">
         <v>2</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="3">
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="3">
         <v>2.5</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E24" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G23" s="17">
-        <v>1</v>
-      </c>
-      <c r="H23" s="3">
+      <c r="G24" s="17">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
         <v>14.52</v>
       </c>
-      <c r="I23" s="17">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="I24" s="17">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
-      <c r="B24" t="s">
+    <row r="25" spans="1:10">
+      <c r="B25" t="s">
         <v>36</v>
       </c>
-      <c r="C24" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="17">
-        <v>1</v>
-      </c>
-      <c r="H24" s="3">
+      <c r="G25" s="17">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
         <v>3.48</v>
       </c>
-      <c r="I24" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="I25" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
         <v>5</v>
       </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="3">
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3">
         <v>3</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E26" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="17">
+      <c r="G26" s="17">
         <v>2</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H26" s="3">
         <v>2.78</v>
       </c>
-      <c r="I25" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="I26" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
         <v>31</v>
       </c>
-      <c r="C26" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3">
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3">
         <v>2</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E27" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G26" s="17">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3">
-        <v>0</v>
-      </c>
-      <c r="I26" s="17">
-        <v>0</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="G27" s="17">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="17">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27">
+    <row r="28" spans="1:10">
+      <c r="A28">
         <v>3</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="3">
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3">
         <v>0.5</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E28" s="3">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G28" s="17">
         <v>5</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H28" s="3">
         <v>5.58</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I28" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="5" customFormat="1">
-      <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28" s="5" t="s">
+    <row r="29" spans="1:10" s="5" customFormat="1">
+      <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="6">
-        <f>0.1*SUM(E2:E27)</f>
+      <c r="D29" s="6">
+        <f>0.1*SUM(E2:E28)</f>
         <v>41.5</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E29" s="6">
         <f t="shared" si="0"/>
         <v>41.5</v>
       </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="18">
-        <v>0</v>
-      </c>
-      <c r="H28" s="6">
-        <v>0</v>
-      </c>
-      <c r="I28" s="18"/>
-    </row>
-    <row r="29" spans="1:10" s="1" customFormat="1">
-      <c r="B29" s="1" t="s">
+      <c r="F29" s="6"/>
+      <c r="G29" s="18">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6">
+        <v>0</v>
+      </c>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:10" s="1" customFormat="1">
+      <c r="B30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2">
-        <f>SUM(E2:E28)</f>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
+        <f>SUM(E2:E29)</f>
         <v>456.5</v>
       </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="2">
-        <f>SUM(H2:H28)</f>
-        <v>436.1694</v>
-      </c>
-      <c r="I29" s="15"/>
-    </row>
-    <row r="30" spans="1:10" s="11" customFormat="1">
-      <c r="A30" s="11">
+      <c r="F30" s="2"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="2">
+        <f>SUM(H2:H29)</f>
+        <v>459.0994</v>
+      </c>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="1:10" s="11" customFormat="1">
+      <c r="A31" s="11">
         <v>2</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B31" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C31" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D31" s="12">
         <v>90</v>
       </c>
-      <c r="E30" s="12">
-        <f t="shared" ref="E30:E35" si="1">A30*D30</f>
+      <c r="E31" s="12">
+        <f t="shared" ref="E31:E36" si="1">A31*D31</f>
         <v>180</v>
       </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="12">
+      <c r="F31" s="12"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="12">
         <v>650</v>
       </c>
-      <c r="I30" s="19"/>
-      <c r="J30" t="s">
+      <c r="I31" s="19"/>
+      <c r="J31" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31">
+    <row r="32" spans="1:10">
+      <c r="A32">
         <v>20</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>47</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D32" s="3">
         <v>10</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E32" s="3">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="H31" s="3">
-        <v>0</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32">
+    <row r="33" spans="1:10">
+      <c r="A33">
         <v>5</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>29</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D33" s="3">
         <v>60</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E33" s="3">
         <f t="shared" si="1"/>
         <v>300</v>
       </c>
-      <c r="G32" s="17">
-        <v>0</v>
-      </c>
-      <c r="H32" s="3">
-        <v>0</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="G33" s="17">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="s">
+    <row r="34" spans="1:10">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
         <v>24</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D34" s="3">
         <v>76</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E34" s="3">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="G33" s="17">
-        <v>0</v>
-      </c>
-      <c r="H33" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" s="11" customFormat="1">
-      <c r="A34" s="7">
-        <v>1</v>
-      </c>
-      <c r="B34" s="7" t="s">
+      <c r="G34" s="17">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="11" customFormat="1">
+      <c r="A35" s="7">
+        <v>1</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C35" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D35" s="12">
         <v>50</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E35" s="12">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="19"/>
-    </row>
-    <row r="35" spans="1:10" s="5" customFormat="1">
-      <c r="A35" s="13">
-        <v>1</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="F35" s="12"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="19"/>
+    </row>
+    <row r="36" spans="1:10" s="5" customFormat="1">
+      <c r="A36" s="13">
+        <v>1</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="6">
-        <f>0.1*SUM(E30:E34)</f>
+      <c r="D36" s="6">
+        <f>0.1*SUM(E31:E35)</f>
         <v>80.600000000000009</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E36" s="6">
         <f t="shared" si="1"/>
         <v>80.600000000000009</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="11" t="s">
+      <c r="F36" s="6"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="9" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B36" s="9" t="s">
+    <row r="37" spans="1:10" s="9" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B37" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10">
-        <f>SUM(E30:E35)</f>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10">
+        <f>SUM(E31:E36)</f>
         <v>886.6</v>
       </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="10">
-        <f>SUM(H30:H35)</f>
+      <c r="F37" s="10"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="10">
+        <f>SUM(H31:H36)</f>
         <v>650</v>
       </c>
-      <c r="I36" s="20"/>
-    </row>
-    <row r="37" spans="1:10" s="1" customFormat="1" ht="15.75" thickTop="1">
-      <c r="B37" s="8" t="s">
+      <c r="I37" s="20"/>
+    </row>
+    <row r="38" spans="1:10" s="1" customFormat="1" ht="15.75" thickTop="1">
+      <c r="B38" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="2">
-        <f>E29+E36</f>
+      <c r="E38" s="2">
+        <f>E30+E37</f>
         <v>1343.1</v>
       </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="2">
-        <f>H29+H36</f>
-        <v>1086.1694</v>
-      </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="1" t="s">
+      <c r="F38" s="2"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="2">
+        <f>H30+H37</f>
+        <v>1109.0994000000001</v>
+      </c>
+      <c r="I38" s="15"/>
+      <c r="J38" s="1" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>